<commit_message>
missing language file info AND adjusted config
</commit_message>
<xml_diff>
--- a/static/config/languageFile.xlsx
+++ b/static/config/languageFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20400"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fenn\Nextcloud\Artikel Cognitive Affective Maps Tools\CAM tools\CAMtools_CAMEL\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fenn\Nextcloud\Artikel Cognitive Affective Maps Tools\CAM tools\CAMtools_CAMEL\static\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC1602C-A6AD-49F2-ABCC-027303E7C34B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86271E35-0185-4172-BC41-A70E75E1AE1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -234,7 +234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G82" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="G83" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -263,7 +263,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="535">
   <si>
     <t>english</t>
   </si>
@@ -1856,6 +1856,18 @@
   </si>
   <si>
     <t>您的CAM已被删除。将没有数据会被保存到服务器。默认CAM已被恢复。</t>
+  </si>
+  <si>
+    <t>popup save button CAM as picture (popSavePicture)</t>
+  </si>
+  <si>
+    <t>popSavePicture_CAM</t>
+  </si>
+  <si>
+    <t>You can save your CAM as a picture (svg file).</t>
+  </si>
+  <si>
+    <t>Sie können Ihr CAM als Bild (svg-Datei) speichern.</t>
   </si>
 </sst>
 </file>
@@ -1897,12 +1909,18 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1917,7 +1935,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1927,6 +1945,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2225,10 +2246,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I89"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I84" sqref="I84"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3858,438 +3879,461 @@
     </row>
     <row r="71" spans="1:7" ht="60">
       <c r="A71" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="60">
+      <c r="A72" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="30">
-      <c r="A72" s="1" t="s">
-        <v>276</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>512</v>
+        <v>518</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="30">
       <c r="A73" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="30">
       <c r="A74" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="30">
       <c r="A75" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="45">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="30">
       <c r="A76" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="60">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="45">
       <c r="A77" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C77" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="60">
+      <c r="A78" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E78" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="F78" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="G77" s="2" t="s">
+      <c r="G78" s="2" t="s">
         <v>516</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="45">
-      <c r="A78" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="45">
       <c r="A79" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>294</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>517</v>
+        <v>339</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="45">
       <c r="A80" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>294</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="45">
       <c r="A81" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>294</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="45">
       <c r="A82" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="45">
+      <c r="A83" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="150">
-      <c r="A83" s="1" t="s">
-        <v>308</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>309</v>
       </c>
       <c r="C83" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="150">
+      <c r="A84" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="D84" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="E83" s="3" t="s">
+      <c r="E84" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="F83" s="3" t="s">
+      <c r="F84" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="G83" s="2" t="s">
+      <c r="G84" s="2" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="75">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:7" ht="75">
+      <c r="A85" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>429</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="G84" s="2" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="90">
-      <c r="A85" s="1" t="s">
-        <v>313</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C85" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="90">
+      <c r="A86" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="D86" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="E85" s="3" t="s">
+      <c r="E86" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="F85" s="3" t="s">
+      <c r="F86" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="G85" s="2" t="s">
+      <c r="G86" s="2" t="s">
         <v>530</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7">
-      <c r="A86" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>321</v>
+        <v>356</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D88" s="2" t="s">
+      <c r="D89" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E88" s="3" t="s">
+      <c r="E89" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="F88" s="3" t="s">
+      <c r="F89" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="G89" s="2" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="30">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:7" ht="30">
+      <c r="A90" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="D89" s="2" t="s">
+      <c r="D90" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="E89" s="3" t="s">
+      <c r="E90" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="F89" s="3" t="s">
+      <c r="F90" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="G89" s="2" t="s">
+      <c r="G90" s="2" t="s">
         <v>526</v>
       </c>
     </row>

</xml_diff>